<commit_message>
Added basic teleop controls
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 20XX.xlsx
+++ b/Kilroy Equipment List 20XX.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="114">
   <si>
     <t>Kilroy Equipment List (20XX)</t>
   </si>
@@ -328,6 +328,42 @@
   </si>
   <si>
     <t>Change Camera Driver Side</t>
+  </si>
+  <si>
+    <t>Left Climb Motor</t>
+  </si>
+  <si>
+    <t>Right Climb Motor</t>
+  </si>
+  <si>
+    <t>Climb Encoder</t>
+  </si>
+  <si>
+    <t>CAN 10</t>
+  </si>
+  <si>
+    <t>CAN 24</t>
+  </si>
+  <si>
+    <t>climbEncoder</t>
+  </si>
+  <si>
+    <t>leftClimbMotor</t>
+  </si>
+  <si>
+    <t>rightClimbMotor</t>
+  </si>
+  <si>
+    <t>Left Drivers Trigger</t>
+  </si>
+  <si>
+    <t>Right Drivers Gear Up</t>
+  </si>
+  <si>
+    <t>Right Driver Trigger</t>
+  </si>
+  <si>
+    <t>Left Driver Trigger</t>
   </si>
 </sst>
 </file>
@@ -499,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -690,6 +726,18 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -698,12 +746,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1022,8 +1064,8 @@
   <dimension ref="A1:AMK241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C80" sqref="C80"/>
+      <pane ySplit="2" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1040,13 +1082,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="25.5">
       <c r="A2" s="5" t="s">
@@ -1068,10 +1110,10 @@
     <row r="3" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="64"/>
+      <c r="D3" s="68"/>
       <c r="E3" s="9" t="s">
         <v>7</v>
       </c>
@@ -1180,16 +1222,28 @@
     <row r="12" spans="1:8" s="4" customFormat="1">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="21"/>
+      <c r="C12" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="66" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="13" spans="1:8" s="4" customFormat="1">
       <c r="A13" s="22"/>
       <c r="B13" s="22"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="17"/>
+      <c r="C13" s="65" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="64" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="14" spans="1:8" s="4" customFormat="1">
       <c r="A14" s="5"/>
@@ -1201,9 +1255,15 @@
     <row r="15" spans="1:8" s="4" customFormat="1">
       <c r="A15" s="22"/>
       <c r="B15" s="22"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="17"/>
+      <c r="C15" s="65" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="67" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="64" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="16" spans="1:8" s="4" customFormat="1">
       <c r="A16" s="5"/>
@@ -1229,10 +1289,10 @@
     <row r="19" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A19" s="38"/>
       <c r="B19" s="38"/>
-      <c r="C19" s="66" t="s">
+      <c r="C19" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="66"/>
+      <c r="D19" s="70"/>
       <c r="E19" s="39" t="s">
         <v>25</v>
       </c>
@@ -1314,10 +1374,10 @@
     <row r="28" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A28" s="38"/>
       <c r="B28" s="38"/>
-      <c r="C28" s="64" t="s">
+      <c r="C28" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="64"/>
+      <c r="D28" s="68"/>
       <c r="E28" s="9" t="s">
         <v>25</v>
       </c>
@@ -1449,10 +1509,10 @@
     <row r="45" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A45" s="38"/>
       <c r="B45" s="38"/>
-      <c r="C45" s="64" t="s">
+      <c r="C45" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="D45" s="64"/>
+      <c r="D45" s="68"/>
       <c r="E45" s="9" t="s">
         <v>33</v>
       </c>
@@ -1496,10 +1556,10 @@
     <row r="50" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A50" s="38"/>
       <c r="B50" s="38"/>
-      <c r="C50" s="64" t="s">
+      <c r="C50" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="D50" s="64"/>
+      <c r="D50" s="68"/>
       <c r="E50" s="9" t="s">
         <v>36</v>
       </c>
@@ -1555,10 +1615,10 @@
     <row r="57" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A57" s="38"/>
       <c r="B57" s="38"/>
-      <c r="C57" s="64" t="s">
+      <c r="C57" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="D57" s="64"/>
+      <c r="D57" s="68"/>
       <c r="E57" s="9" t="s">
         <v>40</v>
       </c>
@@ -1600,10 +1660,10 @@
     <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A62" s="38"/>
       <c r="B62" s="38"/>
-      <c r="C62" s="64" t="s">
+      <c r="C62" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="D62" s="64"/>
+      <c r="D62" s="68"/>
       <c r="E62" s="9" t="s">
         <v>44</v>
       </c>
@@ -1648,10 +1708,10 @@
     <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A68" s="38"/>
       <c r="B68" s="38"/>
-      <c r="C68" s="64" t="s">
+      <c r="C68" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="D68" s="64"/>
+      <c r="D68" s="68"/>
       <c r="E68" s="9" t="s">
         <v>46</v>
       </c>
@@ -1695,10 +1755,10 @@
     <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A73" s="38"/>
       <c r="B73" s="38"/>
-      <c r="C73" s="64" t="s">
+      <c r="C73" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="D73" s="64"/>
+      <c r="D73" s="68"/>
       <c r="E73" s="9" t="s">
         <v>50</v>
       </c>
@@ -1763,10 +1823,10 @@
     <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A78" s="38"/>
       <c r="B78" s="38"/>
-      <c r="C78" s="64" t="s">
+      <c r="C78" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="D78" s="64"/>
+      <c r="D78" s="68"/>
       <c r="E78" s="9" t="s">
         <v>63</v>
       </c>
@@ -1786,27 +1846,35 @@
     <row r="80" spans="1:8" s="54" customFormat="1">
       <c r="A80" s="22"/>
       <c r="B80" s="22"/>
-      <c r="C80" s="68" t="s">
+      <c r="C80" s="65" t="s">
         <v>101</v>
       </c>
       <c r="D80" s="30"/>
-      <c r="E80" s="67" t="s">
+      <c r="E80" s="64" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="81" spans="1:6" s="4" customFormat="1">
       <c r="A81" s="58"/>
       <c r="B81" s="58"/>
-      <c r="C81" s="31"/>
+      <c r="C81" s="33" t="s">
+        <v>110</v>
+      </c>
       <c r="D81" s="31"/>
-      <c r="E81" s="31"/>
+      <c r="E81" s="33" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="82" spans="1:6" s="4" customFormat="1">
       <c r="A82" s="22"/>
       <c r="B82" s="22"/>
-      <c r="C82" s="17"/>
+      <c r="C82" s="64" t="s">
+        <v>111</v>
+      </c>
       <c r="D82" s="30"/>
-      <c r="E82" s="17"/>
+      <c r="E82" s="64" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="83" spans="1:6" s="4" customFormat="1">
       <c r="A83" s="43"/>
@@ -1930,10 +1998,10 @@
     <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A99" s="38"/>
       <c r="B99" s="38"/>
-      <c r="C99" s="64" t="s">
+      <c r="C99" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="D99" s="64"/>
+      <c r="D99" s="68"/>
       <c r="E99" s="9" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Added drive code with gears
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 20XX.xlsx
+++ b/Kilroy Equipment List 20XX.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="118">
   <si>
     <t>Kilroy Equipment List (20XX)</t>
   </si>
@@ -354,9 +354,6 @@
     <t>rightClimbMotor</t>
   </si>
   <si>
-    <t>Left Drivers Trigger</t>
-  </si>
-  <si>
     <t>Right Drivers Gear Up</t>
   </si>
   <si>
@@ -364,6 +361,21 @@
   </si>
   <si>
     <t>Left Driver Trigger</t>
+  </si>
+  <si>
+    <t>driverGearUpPressed</t>
+  </si>
+  <si>
+    <t>driverGearDownPressed</t>
+  </si>
+  <si>
+    <t>Left Drivers Gear Up</t>
+  </si>
+  <si>
+    <t>rightDriverCameraSwitchButtonPressed</t>
+  </si>
+  <si>
+    <t>rightOperatorCameraSwitchButtonPressed</t>
   </si>
 </sst>
 </file>
@@ -738,11 +750,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1053,7 +1065,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1064,8 +1076,8 @@
   <dimension ref="A1:AMK241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E81" sqref="E81"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1082,13 +1094,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="25.5">
       <c r="A2" s="5" t="s">
@@ -1110,10 +1122,10 @@
     <row r="3" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="68"/>
+      <c r="D3" s="69"/>
       <c r="E3" s="9" t="s">
         <v>7</v>
       </c>
@@ -1374,10 +1386,10 @@
     <row r="28" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A28" s="38"/>
       <c r="B28" s="38"/>
-      <c r="C28" s="68" t="s">
+      <c r="C28" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="68"/>
+      <c r="D28" s="69"/>
       <c r="E28" s="9" t="s">
         <v>25</v>
       </c>
@@ -1509,10 +1521,10 @@
     <row r="45" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A45" s="38"/>
       <c r="B45" s="38"/>
-      <c r="C45" s="68" t="s">
+      <c r="C45" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="D45" s="68"/>
+      <c r="D45" s="69"/>
       <c r="E45" s="9" t="s">
         <v>33</v>
       </c>
@@ -1556,10 +1568,10 @@
     <row r="50" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A50" s="38"/>
       <c r="B50" s="38"/>
-      <c r="C50" s="68" t="s">
+      <c r="C50" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="D50" s="68"/>
+      <c r="D50" s="69"/>
       <c r="E50" s="9" t="s">
         <v>36</v>
       </c>
@@ -1615,10 +1627,10 @@
     <row r="57" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A57" s="38"/>
       <c r="B57" s="38"/>
-      <c r="C57" s="68" t="s">
+      <c r="C57" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="D57" s="68"/>
+      <c r="D57" s="69"/>
       <c r="E57" s="9" t="s">
         <v>40</v>
       </c>
@@ -1660,10 +1672,10 @@
     <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A62" s="38"/>
       <c r="B62" s="38"/>
-      <c r="C62" s="68" t="s">
+      <c r="C62" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="D62" s="68"/>
+      <c r="D62" s="69"/>
       <c r="E62" s="9" t="s">
         <v>44</v>
       </c>
@@ -1708,10 +1720,10 @@
     <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A68" s="38"/>
       <c r="B68" s="38"/>
-      <c r="C68" s="68" t="s">
+      <c r="C68" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="D68" s="68"/>
+      <c r="D68" s="69"/>
       <c r="E68" s="9" t="s">
         <v>46</v>
       </c>
@@ -1755,10 +1767,10 @@
     <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A73" s="38"/>
       <c r="B73" s="38"/>
-      <c r="C73" s="68" t="s">
+      <c r="C73" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="D73" s="68"/>
+      <c r="D73" s="69"/>
       <c r="E73" s="9" t="s">
         <v>50</v>
       </c>
@@ -1823,33 +1835,37 @@
     <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A78" s="38"/>
       <c r="B78" s="38"/>
-      <c r="C78" s="68" t="s">
+      <c r="C78" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="D78" s="68"/>
+      <c r="D78" s="69"/>
       <c r="E78" s="9" t="s">
         <v>63</v>
       </c>
       <c r="G78" s="56"/>
     </row>
-    <row r="79" spans="1:8" s="4" customFormat="1">
+    <row r="79" spans="1:8" s="4" customFormat="1" ht="25.5">
       <c r="A79" s="18"/>
       <c r="B79" s="18"/>
       <c r="C79" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="D79" s="34"/>
+      <c r="D79" s="34" t="s">
+        <v>117</v>
+      </c>
       <c r="E79" s="33" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="80" spans="1:8" s="54" customFormat="1">
+    <row r="80" spans="1:8" s="54" customFormat="1" ht="25.5">
       <c r="A80" s="22"/>
       <c r="B80" s="22"/>
       <c r="C80" s="65" t="s">
         <v>101</v>
       </c>
-      <c r="D80" s="30"/>
+      <c r="D80" s="67" t="s">
+        <v>116</v>
+      </c>
       <c r="E80" s="64" t="s">
         <v>100</v>
       </c>
@@ -1858,22 +1874,26 @@
       <c r="A81" s="58"/>
       <c r="B81" s="58"/>
       <c r="C81" s="33" t="s">
-        <v>110</v>
-      </c>
-      <c r="D81" s="31"/>
+        <v>115</v>
+      </c>
+      <c r="D81" s="33" t="s">
+        <v>114</v>
+      </c>
       <c r="E81" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="82" spans="1:6" s="4" customFormat="1">
       <c r="A82" s="22"/>
       <c r="B82" s="22"/>
       <c r="C82" s="64" t="s">
+        <v>110</v>
+      </c>
+      <c r="D82" s="67" t="s">
+        <v>113</v>
+      </c>
+      <c r="E82" s="64" t="s">
         <v>111</v>
-      </c>
-      <c r="D82" s="30"/>
-      <c r="E82" s="64" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="83" spans="1:6" s="4" customFormat="1">
@@ -1998,10 +2018,10 @@
     <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A99" s="38"/>
       <c r="B99" s="38"/>
-      <c r="C99" s="68" t="s">
+      <c r="C99" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="D99" s="68"/>
+      <c r="D99" s="69"/>
       <c r="E99" s="9" t="s">
         <v>63</v>
       </c>
@@ -3079,11 +3099,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C45:D45"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C99:D99"/>
     <mergeCell ref="C50:D50"/>
@@ -3091,6 +3106,11 @@
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C73:D73"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Added climb servo and corrected left top motor
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 20XX.xlsx
+++ b/Kilroy Equipment List 20XX.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="121">
   <si>
     <t>Kilroy Equipment List (20XX)</t>
   </si>
@@ -54,36 +54,24 @@
     <t>leftFrontMotor</t>
   </si>
   <si>
-    <t>CAN 0</t>
-  </si>
-  <si>
     <t>Right Front Motor (controller_type)</t>
   </si>
   <si>
     <t>rightFrontMotor</t>
   </si>
   <si>
-    <t>CAN 1</t>
-  </si>
-  <si>
     <t>Left Rear Motor (controller_type)</t>
   </si>
   <si>
     <t>leftRearMotor</t>
   </si>
   <si>
-    <t>CAN 2</t>
-  </si>
-  <si>
     <t>Right Rear Motor (controller_type)</t>
   </si>
   <si>
     <t>rightRearMotor</t>
   </si>
   <si>
-    <t>CAN 3</t>
-  </si>
-  <si>
     <t>Left Drive Encoder</t>
   </si>
   <si>
@@ -376,6 +364,27 @@
   </si>
   <si>
     <t>rightOperatorCameraSwitchButtonPressed</t>
+  </si>
+  <si>
+    <t>CAN 12</t>
+  </si>
+  <si>
+    <t>CAN 15</t>
+  </si>
+  <si>
+    <t>CAN 14</t>
+  </si>
+  <si>
+    <t>CAN 6</t>
+  </si>
+  <si>
+    <t>Climb Servo</t>
+  </si>
+  <si>
+    <t>climbServo</t>
+  </si>
+  <si>
+    <t>PWM 2</t>
   </si>
 </sst>
 </file>
@@ -547,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -750,14 +759,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1065,7 +1077,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1076,8 +1088,8 @@
   <dimension ref="A1:AMK241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D80" sqref="D80"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1094,13 +1106,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="25.5">
       <c r="A2" s="5" t="s">
@@ -1122,10 +1134,10 @@
     <row r="3" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="69"/>
+      <c r="D3" s="68"/>
       <c r="E3" s="9" t="s">
         <v>7</v>
       </c>
@@ -1139,47 +1151,47 @@
       <c r="D4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>10</v>
+      <c r="E4" s="66" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>13</v>
+      <c r="E5" s="64" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A6" s="18"/>
       <c r="B6" s="18"/>
       <c r="C6" s="19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="E6" s="66" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="23" customFormat="1">
       <c r="A7" s="22"/>
       <c r="B7" s="22"/>
       <c r="C7" s="15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="E7" s="64" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1">
@@ -1196,13 +1208,13 @@
       <c r="A9" s="22"/>
       <c r="B9" s="22"/>
       <c r="C9" s="29" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
@@ -1212,13 +1224,13 @@
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="31" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
@@ -1235,54 +1247,60 @@
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="33" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E12" s="66" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="4" customFormat="1">
       <c r="A13" s="22"/>
       <c r="B13" s="22"/>
       <c r="C13" s="65" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D13" s="67" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E13" s="64" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="4" customFormat="1">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="35"/>
+      <c r="C14" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" s="71" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="15" spans="1:8" s="4" customFormat="1">
       <c r="A15" s="22"/>
       <c r="B15" s="22"/>
-      <c r="C15" s="65" t="s">
-        <v>104</v>
-      </c>
-      <c r="D15" s="67" t="s">
-        <v>107</v>
-      </c>
-      <c r="E15" s="64" t="s">
-        <v>105</v>
-      </c>
+      <c r="C15" s="65"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="64"/>
     </row>
     <row r="16" spans="1:8" s="4" customFormat="1">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="21"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="65" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="64" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="17" spans="1:8" s="4" customFormat="1">
       <c r="A17" s="22"/>
@@ -1302,11 +1320,11 @@
       <c r="A19" s="38"/>
       <c r="B19" s="38"/>
       <c r="C19" s="70" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D19" s="70"/>
       <c r="E19" s="39" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="4" customFormat="1">
@@ -1386,38 +1404,38 @@
     <row r="28" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A28" s="38"/>
       <c r="B28" s="38"/>
-      <c r="C28" s="69" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="69"/>
+      <c r="C28" s="68" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="68"/>
       <c r="E28" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="4" customFormat="1">
       <c r="A29" s="41"/>
       <c r="B29" s="41"/>
       <c r="C29" s="29" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D29" s="44" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="4" customFormat="1">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="31" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="4" customFormat="1">
@@ -1521,20 +1539,20 @@
     <row r="45" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A45" s="38"/>
       <c r="B45" s="38"/>
-      <c r="C45" s="69" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" s="69"/>
+      <c r="C45" s="68" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" s="68"/>
       <c r="E45" s="9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:5" s="4" customFormat="1">
       <c r="A46" s="47" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B46" s="47" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C46" s="29"/>
       <c r="D46" s="48"/>
@@ -1549,10 +1567,10 @@
     </row>
     <row r="48" spans="1:5" s="4" customFormat="1">
       <c r="A48" s="22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C48" s="29"/>
       <c r="D48" s="30"/>
@@ -1568,25 +1586,25 @@
     <row r="50" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A50" s="38"/>
       <c r="B50" s="38"/>
-      <c r="C50" s="69" t="s">
-        <v>35</v>
-      </c>
-      <c r="D50" s="69"/>
+      <c r="C50" s="68" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" s="68"/>
       <c r="E50" s="9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:5" s="46" customFormat="1" ht="13.15" customHeight="1">
       <c r="A51" s="52"/>
       <c r="B51" s="52"/>
       <c r="C51" s="53" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D51" s="48" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E51" s="49" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:5" s="4" customFormat="1">
@@ -1627,25 +1645,25 @@
     <row r="57" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A57" s="38"/>
       <c r="B57" s="38"/>
-      <c r="C57" s="69" t="s">
-        <v>39</v>
-      </c>
-      <c r="D57" s="69"/>
+      <c r="C57" s="68" t="s">
+        <v>35</v>
+      </c>
+      <c r="D57" s="68"/>
       <c r="E57" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="46" customFormat="1" ht="13.15" customHeight="1">
       <c r="A58" s="52"/>
       <c r="B58" s="52"/>
       <c r="C58" s="53" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D58" s="48" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E58" s="49" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="4" customFormat="1">
@@ -1672,12 +1690,12 @@
     <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A62" s="38"/>
       <c r="B62" s="38"/>
-      <c r="C62" s="69" t="s">
-        <v>43</v>
-      </c>
-      <c r="D62" s="69"/>
+      <c r="C62" s="68" t="s">
+        <v>39</v>
+      </c>
+      <c r="D62" s="68"/>
       <c r="E62" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="63" spans="1:5" s="4" customFormat="1">
@@ -1720,25 +1738,25 @@
     <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A68" s="38"/>
       <c r="B68" s="38"/>
-      <c r="C68" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="D68" s="69"/>
+      <c r="C68" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="D68" s="68"/>
       <c r="E68" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="4" customFormat="1">
       <c r="A69" s="18"/>
       <c r="B69" s="18"/>
       <c r="C69" s="42" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D69" s="43" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E69" s="13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="70" spans="1:8" s="4" customFormat="1">
@@ -1767,12 +1785,12 @@
     <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A73" s="38"/>
       <c r="B73" s="38"/>
-      <c r="C73" s="69" t="s">
-        <v>49</v>
-      </c>
-      <c r="D73" s="69"/>
+      <c r="C73" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="D73" s="68"/>
       <c r="E73" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G73" s="56"/>
     </row>
@@ -1780,13 +1798,13 @@
       <c r="A74" s="18"/>
       <c r="B74" s="18"/>
       <c r="C74" s="33" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D74" s="34" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E74" s="13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G74" s="56"/>
     </row>
@@ -1794,13 +1812,13 @@
       <c r="A75" s="22"/>
       <c r="B75" s="22"/>
       <c r="C75" s="29" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D75" s="30" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E75" s="17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G75" s="56"/>
     </row>
@@ -1808,13 +1826,13 @@
       <c r="A76" s="18"/>
       <c r="B76" s="18"/>
       <c r="C76" s="31" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D76" s="32" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E76" s="21" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G76" s="56"/>
     </row>
@@ -1822,25 +1840,25 @@
       <c r="A77" s="22"/>
       <c r="B77" s="22"/>
       <c r="C77" s="29" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D77" s="30" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E77" s="17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G77" s="56"/>
     </row>
     <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A78" s="38"/>
       <c r="B78" s="38"/>
-      <c r="C78" s="69" t="s">
-        <v>62</v>
-      </c>
-      <c r="D78" s="69"/>
+      <c r="C78" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="D78" s="68"/>
       <c r="E78" s="9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G78" s="56"/>
     </row>
@@ -1848,52 +1866,52 @@
       <c r="A79" s="18"/>
       <c r="B79" s="18"/>
       <c r="C79" s="57" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D79" s="34" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E79" s="33" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="54" customFormat="1" ht="25.5">
       <c r="A80" s="22"/>
       <c r="B80" s="22"/>
       <c r="C80" s="65" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D80" s="67" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E80" s="64" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="81" spans="1:6" s="4" customFormat="1">
       <c r="A81" s="58"/>
       <c r="B81" s="58"/>
       <c r="C81" s="33" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D81" s="33" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E81" s="33" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="82" spans="1:6" s="4" customFormat="1">
       <c r="A82" s="22"/>
       <c r="B82" s="22"/>
       <c r="C82" s="64" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D82" s="67" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E82" s="64" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="83" spans="1:6" s="4" customFormat="1">
@@ -2018,12 +2036,12 @@
     <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A99" s="38"/>
       <c r="B99" s="38"/>
-      <c r="C99" s="69" t="s">
-        <v>64</v>
-      </c>
-      <c r="D99" s="69"/>
+      <c r="C99" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="D99" s="68"/>
       <c r="E99" s="9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G99" s="56"/>
     </row>
@@ -2031,13 +2049,13 @@
       <c r="A100" s="18"/>
       <c r="B100" s="18"/>
       <c r="C100" s="57" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D100" s="43" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E100" s="42" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="101" spans="1:7" s="4" customFormat="1">
@@ -2051,11 +2069,11 @@
       <c r="A102" s="38"/>
       <c r="B102" s="38"/>
       <c r="C102" s="39" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D102" s="60"/>
       <c r="E102" s="39" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="103" spans="1:7" s="4" customFormat="1">
@@ -2069,39 +2087,39 @@
       <c r="A104" s="22"/>
       <c r="B104" s="22"/>
       <c r="C104" s="29" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D104" s="30" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E104" s="17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="105" spans="1:7" s="4" customFormat="1">
       <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="42" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D105" s="34" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E105" s="61" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="106" spans="1:7" s="4" customFormat="1">
       <c r="A106" s="22"/>
       <c r="B106" s="22"/>
       <c r="C106" s="29" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D106" s="30" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E106" s="62" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="107" spans="1:7" s="4" customFormat="1">
@@ -2115,78 +2133,78 @@
       <c r="A108" s="22"/>
       <c r="B108" s="22"/>
       <c r="C108" s="29" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D108" s="30" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E108" s="17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="109" spans="1:7" s="4" customFormat="1">
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="31" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D109" s="32" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E109" s="21" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="110" spans="1:7" s="4" customFormat="1">
       <c r="A110" s="22"/>
       <c r="B110" s="22"/>
       <c r="C110" s="29" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D110" s="30" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E110" s="17" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="111" spans="1:7" s="4" customFormat="1">
       <c r="A111" s="5"/>
       <c r="B111" s="5"/>
       <c r="C111" s="31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D111" s="32" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E111" s="31" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="112" spans="1:7" s="4" customFormat="1">
       <c r="A112" s="22"/>
       <c r="B112" s="22"/>
       <c r="C112" s="29" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D112" s="30" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E112" s="17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="113" spans="1:5" s="4" customFormat="1">
       <c r="A113" s="5"/>
       <c r="B113" s="5"/>
       <c r="C113" s="31" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D113" s="32" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E113" s="21" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="114" spans="1:5" s="4" customFormat="1">
@@ -2200,26 +2218,26 @@
       <c r="A115" s="5"/>
       <c r="B115" s="5"/>
       <c r="C115" s="31" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D115" s="32" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E115" s="31" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="116" spans="1:5" s="4" customFormat="1">
       <c r="A116" s="22"/>
       <c r="B116" s="22"/>
       <c r="C116" s="29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D116" s="30" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E116" s="17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="117" spans="1:5" s="4" customFormat="1">
@@ -3099,6 +3117,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C45:D45"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C99:D99"/>
     <mergeCell ref="C50:D50"/>
@@ -3106,11 +3129,6 @@
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C73:D73"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Addded Red Lights onto equitment list needs tested
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 20XX.xlsx
+++ b/Kilroy Equipment List 20XX.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="129">
   <si>
     <t>Kilroy Equipment List (20XX)</t>
   </si>
@@ -385,6 +385,30 @@
   </si>
   <si>
     <t>PWM 2</t>
+  </si>
+  <si>
+    <t>Red Light Launcher Sensor 4</t>
+  </si>
+  <si>
+    <t>Red Light Launcher Sensor 3</t>
+  </si>
+  <si>
+    <t>Red Light Launcher Sensor 2</t>
+  </si>
+  <si>
+    <t>Red Light Launcher Sensor 1</t>
+  </si>
+  <si>
+    <t>DIO 11</t>
+  </si>
+  <si>
+    <t>DIO 13</t>
+  </si>
+  <si>
+    <t>DIO14</t>
+  </si>
+  <si>
+    <t>DIO 12</t>
   </si>
 </sst>
 </file>
@@ -759,17 +783,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1077,7 +1101,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1087,9 +1111,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1134,10 +1158,10 @@
     <row r="3" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="68"/>
+      <c r="D3" s="70"/>
       <c r="E3" s="9" t="s">
         <v>7</v>
       </c>
@@ -1278,7 +1302,7 @@
       <c r="D14" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="E14" s="71" t="s">
+      <c r="E14" s="68" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1319,10 +1343,10 @@
     <row r="19" spans="1:8" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A19" s="38"/>
       <c r="B19" s="38"/>
-      <c r="C19" s="70" t="s">
+      <c r="C19" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="70"/>
+      <c r="D19" s="71"/>
       <c r="E19" s="39" t="s">
         <v>21</v>
       </c>
@@ -1330,23 +1354,35 @@
     <row r="20" spans="1:8" s="4" customFormat="1">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
-      <c r="C20" s="29"/>
+      <c r="C20" s="65" t="s">
+        <v>124</v>
+      </c>
       <c r="D20" s="30"/>
-      <c r="E20" s="17"/>
+      <c r="E20" s="64" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="21" spans="1:8" s="4" customFormat="1">
       <c r="A21" s="40"/>
       <c r="B21" s="40"/>
-      <c r="C21" s="33"/>
+      <c r="C21" s="33" t="s">
+        <v>123</v>
+      </c>
       <c r="D21" s="34"/>
-      <c r="E21" s="21"/>
+      <c r="E21" s="66" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="22" spans="1:8" s="4" customFormat="1">
       <c r="A22" s="22"/>
       <c r="B22" s="22"/>
-      <c r="C22" s="29"/>
+      <c r="C22" s="65" t="s">
+        <v>122</v>
+      </c>
       <c r="D22" s="30"/>
-      <c r="E22" s="17"/>
+      <c r="E22" s="64" t="s">
+        <v>125</v>
+      </c>
       <c r="F22" s="28"/>
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
@@ -1354,9 +1390,13 @@
     <row r="23" spans="1:8" s="4" customFormat="1">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
-      <c r="C23" s="33"/>
+      <c r="C23" s="33" t="s">
+        <v>121</v>
+      </c>
       <c r="D23" s="34"/>
-      <c r="E23" s="13"/>
+      <c r="E23" s="66" t="s">
+        <v>127</v>
+      </c>
       <c r="F23" s="28"/>
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
@@ -1404,10 +1444,10 @@
     <row r="28" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A28" s="38"/>
       <c r="B28" s="38"/>
-      <c r="C28" s="68" t="s">
+      <c r="C28" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="68"/>
+      <c r="D28" s="70"/>
       <c r="E28" s="9" t="s">
         <v>21</v>
       </c>
@@ -1539,10 +1579,10 @@
     <row r="45" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A45" s="38"/>
       <c r="B45" s="38"/>
-      <c r="C45" s="68" t="s">
+      <c r="C45" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="D45" s="68"/>
+      <c r="D45" s="70"/>
       <c r="E45" s="9" t="s">
         <v>29</v>
       </c>
@@ -1586,10 +1626,10 @@
     <row r="50" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A50" s="38"/>
       <c r="B50" s="38"/>
-      <c r="C50" s="68" t="s">
+      <c r="C50" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="D50" s="68"/>
+      <c r="D50" s="70"/>
       <c r="E50" s="9" t="s">
         <v>32</v>
       </c>
@@ -1645,10 +1685,10 @@
     <row r="57" spans="1:5" s="4" customFormat="1" ht="13.15" customHeight="1">
       <c r="A57" s="38"/>
       <c r="B57" s="38"/>
-      <c r="C57" s="68" t="s">
+      <c r="C57" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="D57" s="68"/>
+      <c r="D57" s="70"/>
       <c r="E57" s="9" t="s">
         <v>36</v>
       </c>
@@ -1690,10 +1730,10 @@
     <row r="62" spans="1:5" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A62" s="38"/>
       <c r="B62" s="38"/>
-      <c r="C62" s="68" t="s">
+      <c r="C62" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="D62" s="68"/>
+      <c r="D62" s="70"/>
       <c r="E62" s="9" t="s">
         <v>40</v>
       </c>
@@ -1738,10 +1778,10 @@
     <row r="68" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A68" s="38"/>
       <c r="B68" s="38"/>
-      <c r="C68" s="68" t="s">
+      <c r="C68" s="70" t="s">
         <v>41</v>
       </c>
-      <c r="D68" s="68"/>
+      <c r="D68" s="70"/>
       <c r="E68" s="9" t="s">
         <v>42</v>
       </c>
@@ -1785,10 +1825,10 @@
     <row r="73" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A73" s="38"/>
       <c r="B73" s="38"/>
-      <c r="C73" s="68" t="s">
+      <c r="C73" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="D73" s="68"/>
+      <c r="D73" s="70"/>
       <c r="E73" s="9" t="s">
         <v>46</v>
       </c>
@@ -1853,10 +1893,10 @@
     <row r="78" spans="1:8" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A78" s="38"/>
       <c r="B78" s="38"/>
-      <c r="C78" s="68" t="s">
+      <c r="C78" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="D78" s="68"/>
+      <c r="D78" s="70"/>
       <c r="E78" s="9" t="s">
         <v>59</v>
       </c>
@@ -2036,10 +2076,10 @@
     <row r="99" spans="1:7" s="4" customFormat="1" ht="13.35" customHeight="1">
       <c r="A99" s="38"/>
       <c r="B99" s="38"/>
-      <c r="C99" s="68" t="s">
+      <c r="C99" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="D99" s="68"/>
+      <c r="D99" s="70"/>
       <c r="E99" s="9" t="s">
         <v>59</v>
       </c>
@@ -3117,11 +3157,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C45:D45"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C99:D99"/>
     <mergeCell ref="C50:D50"/>
@@ -3129,6 +3164,11 @@
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C73:D73"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.5" bottom="0.25" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Added BallHandler Class + equipment list stuff
</commit_message>
<xml_diff>
--- a/Kilroy Equipment List 20XX.xlsx
+++ b/Kilroy Equipment List 20XX.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="133">
   <si>
     <t>Kilroy Equipment List (20XX)</t>
   </si>
@@ -399,16 +399,28 @@
     <t>Red Light Launcher Sensor 1</t>
   </si>
   <si>
-    <t>DIO 11</t>
-  </si>
-  <si>
-    <t>DIO 13</t>
-  </si>
-  <si>
-    <t>DIO14</t>
-  </si>
-  <si>
-    <t>DIO 12</t>
+    <t>ballPickup1</t>
+  </si>
+  <si>
+    <t>ballPickup2</t>
+  </si>
+  <si>
+    <t>ballPickup3</t>
+  </si>
+  <si>
+    <t>ballpickup4</t>
+  </si>
+  <si>
+    <t>DIO 24</t>
+  </si>
+  <si>
+    <t>DIO 23</t>
+  </si>
+  <si>
+    <t>DIO 22</t>
+  </si>
+  <si>
+    <t>DIO 21</t>
   </si>
 </sst>
 </file>
@@ -1112,8 +1124,8 @@
   <dimension ref="A1:AMK241"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -1357,9 +1369,11 @@
       <c r="C20" s="65" t="s">
         <v>124</v>
       </c>
-      <c r="D20" s="30"/>
+      <c r="D20" s="67" t="s">
+        <v>125</v>
+      </c>
       <c r="E20" s="64" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="4" customFormat="1">
@@ -1368,9 +1382,11 @@
       <c r="C21" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="34"/>
+      <c r="D21" s="34" t="s">
+        <v>126</v>
+      </c>
       <c r="E21" s="66" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="4" customFormat="1">
@@ -1379,9 +1395,11 @@
       <c r="C22" s="65" t="s">
         <v>122</v>
       </c>
-      <c r="D22" s="30"/>
+      <c r="D22" s="67" t="s">
+        <v>127</v>
+      </c>
       <c r="E22" s="64" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="F22" s="28"/>
       <c r="G22" s="28"/>
@@ -1393,9 +1411,11 @@
       <c r="C23" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="D23" s="34"/>
+      <c r="D23" s="34" t="s">
+        <v>128</v>
+      </c>
       <c r="E23" s="66" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F23" s="28"/>
       <c r="G23" s="28"/>

</xml_diff>